<commit_message>
FEAT: Modifying dimensions for Slowly Changing Dimensions types
</commit_message>
<xml_diff>
--- a/files/DIMENSAO.xlsx
+++ b/files/DIMENSAO.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\BI-DW-with-Pentaho\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0219532E-F223-4A9C-8973-11B058928796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259CE435-94E5-49B5-8DA5-52786D5C7959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{77FE4DFA-C449-48DE-9648-46C8DF06C3B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{77FE4DFA-C449-48DE-9648-46C8DF06C3B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>CODIGO</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>5288954</t>
+  </si>
+  <si>
+    <t>RS</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>